<commit_message>
[FE-Add] Import Product, Strategy
</commit_message>
<xml_diff>
--- a/budgetin/api/utils/template/import_template_product.xlsx
+++ b/budgetin/api/utils/template/import_template_product.xlsx
@@ -560,7 +560,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -588,255 +588,357 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ASET ROA TANAH</t>
+          <t>Keperluan Komputer</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Hyperion ASET ROA TANAH</t>
+          <t>Keperluan Komputer</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>COA untuk ASET ROA TANAH</t>
+          <t>COA untuk Keperluan Komputer</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Biaya Pengelola Pendukung Operasional</t>
+          <t>M. HW</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Hyperion Biaya Pengelola Pendukung Operasional</t>
+          <t>Maintenance Hardware</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>COA untuk Biaya Pengelola Pendukung Operasional</t>
+          <t>COA untuk Maintenance Hardware</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Biaya Pengelola Pendukung Proses</t>
+          <t>Test COA</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Hyperion Biaya Pengelola Pendukung Proses</t>
+          <t>Hype COA</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>COA untuk Biaya Pengelola Pendukung Proses</t>
+          <t>Def COA</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Consultant</t>
+          <t>Coa 1</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Hyperion Consultant</t>
+          <t>Coa 3</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>COA untuk Consultant</t>
+          <t>Coa 2</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Gedung</t>
+          <t>Coa 2</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Hyperion Gedung</t>
+          <t>Coa 2</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>COA untuk Gedung</t>
+          <t>Coa 2</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>HW</t>
+          <t>Coa 3</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Hyperion HW</t>
+          <t>Coa 3</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>COA untuk HW</t>
+          <t>Coa 3</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Keperluan Kantor Lainnya</t>
+          <t>Coa 4</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Hyperion Keperluan Kantor Lainnya</t>
+          <t>Coa 4</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>COA untuk Keperluan Kantor Lainnya</t>
+          <t>Coa 4</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Keperluan Komputer</t>
+          <t>Coa 5</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Hyperion Keperluan Komputer</t>
+          <t>Coa 5</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>COA untuk Keperluan Komputer</t>
+          <t>Coa 5</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>M. HW</t>
+          <t>Gedung</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Hyperion M. HW</t>
+          <t>Gedung Hyperion</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>COA untuk M. HW</t>
+          <t>COA untuk Gedung</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>M. SW</t>
+          <t>ASET ROA TANAH</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Hyperion M. SW</t>
+          <t>ROA</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>COA untuk M. SW</t>
+          <t>COA untuk Roa Tanah</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Pemanfaatan IT</t>
+          <t>Pemeliharaan Gedung &amp; Perabotan</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Hyperion Pemanfaatan IT</t>
+          <t>M.Gedung&amp;Perabotan</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>COA untuk Pemanfaatan IT</t>
+          <t>COA untuk Maintenance Gedung &amp; Perabotan</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Pemeliharaan Gedung &amp; Perabotan</t>
+          <t>SW</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Hyperion Pemeliharaan Gedung &amp; Perabotan</t>
+          <t>Software</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>COA untuk Pemeliharaan Gedung &amp; Perabotan</t>
+          <t>COA untuk Software</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Promosi</t>
+          <t>HW</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Hyperion Promosi</t>
+          <t>Hardware</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>COA untuk Promosi</t>
+          <t>COA untuk Hardware</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Sewa Gedung</t>
+          <t>M. SW</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Hyperion Sewa Gedung</t>
+          <t>Maintenance Software</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>COA untuk Sewa Gedung</t>
+          <t>COA untuk Maintenance Software</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>SW</t>
+          <t>Consultant</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Hyperion SW</t>
+          <t>Consultant</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>COA untuk SW</t>
+          <t>COA untuk Consultant</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Pemanfaatan IT</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Pemanfaatan IT</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>COA untuk pemanfaatan IT</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Sewa Gedung</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Sewa Gedung</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>COA untuk Sewa Gedung</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Keperluan Kantor Lainnya</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Miscellaneous</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>COA untuk keperluan kantor lainnya</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Biaya Pengelola Pendukung Operasional</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Biaya Pengelola Pendukung Operator</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>COA Pendukung Operator</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Promosi</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Promosi</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>COA untuk Promosi</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Biaya Pengelola Pendukung Proses</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Pengelola Pendukung Proses</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>COA untuk Biaya Pengelola Pendukung Proses</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
[BE-Edit] Export budget, and import product
</commit_message>
<xml_diff>
--- a/budgetin/api/utils/template/import_template_product.xlsx
+++ b/budgetin/api/utils/template/import_template_product.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="product" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="example" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="existing_coa" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="existing_strategy" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -18,18 +18,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <b val="1"/>
-      <sz val="11"/>
     </font>
     <font>
       <b val="1"/>
@@ -43,27 +38,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -76,12 +56,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -429,15 +406,15 @@
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col width="13.33203125" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="58.6640625" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="17.5546875" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="13.28515625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="58.7109375" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="17.5703125" bestFit="1" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -470,15 +447,15 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col width="13.33203125" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="58.6640625" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="17.5546875" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="13.28515625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="58.7109375" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="17.5703125" bestFit="1" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -560,7 +537,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -569,376 +546,37 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
-        <is>
-          <t>coa_name</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>hyperion_name</t>
-        </is>
-      </c>
-      <c r="C1" s="2" t="inlineStr">
-        <is>
-          <t>coa_definition</t>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>strategy_name</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Keperluan Komputer</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Keperluan Komputer</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>COA untuk Keperluan Komputer</t>
+          <t>Grow the Business</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>M. HW</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Maintenance Hardware</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>COA untuk Maintenance Hardware</t>
+          <t>Strategy 1</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Test COA</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Hype COA</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Def COA</t>
+          <t>Run the Business</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Coa 1</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Coa 3</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Coa 2</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Coa 2</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Coa 2</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Coa 2</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Coa 3</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Coa 3</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Coa 3</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Coa 4</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Coa 4</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Coa 4</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Coa 5</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Coa 5</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Coa 5</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Gedung</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Gedung Hyperion</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>COA untuk Gedung</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>ASET ROA TANAH</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>ROA</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>COA untuk Roa Tanah</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Pemeliharaan Gedung &amp; Perabotan</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>M.Gedung&amp;Perabotan</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>COA untuk Maintenance Gedung &amp; Perabotan</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>SW</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Software</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>COA untuk Software</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>HW</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Hardware</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>COA untuk Hardware</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>M. SW</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Maintenance Software</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>COA untuk Maintenance Software</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Consultant</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Consultant</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>COA untuk Consultant</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Pemanfaatan IT</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Pemanfaatan IT</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>COA untuk pemanfaatan IT</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Sewa Gedung</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Sewa Gedung</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>COA untuk Sewa Gedung</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Keperluan Kantor Lainnya</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Miscellaneous</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>COA untuk keperluan kantor lainnya</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Biaya Pengelola Pendukung Operasional</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Biaya Pengelola Pendukung Operator</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>COA Pendukung Operator</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Promosi</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Promosi</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>COA untuk Promosi</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Biaya Pengelola Pendukung Proses</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Pengelola Pendukung Proses</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>COA untuk Biaya Pengelola Pendukung Proses</t>
+          <t>Strategy 2</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
[FE-Edit] Download Product Template from Backend
</commit_message>
<xml_diff>
--- a/budgetin/api/utils/template/import_template_product.xlsx
+++ b/budgetin/api/utils/template/import_template_product.xlsx
@@ -9,6 +9,7 @@
     <sheet name="product" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="example" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="existing_coa" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="existing_strategy" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -945,4 +946,58 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>strategy_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Grow the Business</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Strategy 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Run the Business</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Strategy 2</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[FE-Edit] Fix Master COA,PRODUCT,STRATEGY,EMPLOYEE,USER
</commit_message>
<xml_diff>
--- a/budgetin/api/utils/template/import_template_product.xlsx
+++ b/budgetin/api/utils/template/import_template_product.xlsx
@@ -954,7 +954,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -997,6 +997,20 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Strategy 321</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Strategy 4</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>